<commit_message>
se crea la base de nacionalidades y entrenadores
</commit_message>
<xml_diff>
--- a/Mundial_Historic_RawData.xlsx
+++ b/Mundial_Historic_RawData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos\Documentos\WILSON\GIT_HUB\futbol_players_scrapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos\Documentos\WILSON\GIT_HUB\Proyecto_MUNDIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2955027E-D05C-47FB-B1DB-8643D3004987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5DC4C4-B654-4D98-9673-928D88929662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{269563F6-9E00-44CA-BA10-A5F5E1FC2A0D}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17257" uniqueCount="4161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17260" uniqueCount="4161">
   <si>
     <t>Año</t>
   </si>
@@ -12517,7 +12517,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12537,6 +12537,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -12574,7 +12580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -12583,6 +12589,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12919,7 +12928,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -27309,6 +27318,9 @@
       <c r="J386" t="s">
         <v>22</v>
       </c>
+      <c r="L386" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A387">
@@ -45828,7 +45840,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="880" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A880" s="4">
         <v>1950</v>
       </c>
@@ -45866,7 +45878,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="881" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A881" s="4">
         <v>1950</v>
       </c>
@@ -45904,7 +45916,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="882" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A882" s="4">
         <v>1950</v>
       </c>
@@ -45942,7 +45954,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="883" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A883" s="4">
         <v>1950</v>
       </c>
@@ -45980,7 +45992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="884" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A884" s="4">
         <v>1950</v>
       </c>
@@ -46018,7 +46030,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="885" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A885" s="4">
         <v>1950</v>
       </c>
@@ -46056,7 +46068,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="886" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A886" s="4">
         <v>1950</v>
       </c>
@@ -46094,7 +46106,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="887" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A887" s="4">
         <v>1950</v>
       </c>
@@ -46132,7 +46144,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="888" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A888" s="4">
         <v>1950</v>
       </c>
@@ -46170,7 +46182,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="889" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A889" s="4">
         <v>1950</v>
       </c>
@@ -46208,7 +46220,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="890" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A890" s="4">
         <v>1950</v>
       </c>
@@ -46246,7 +46258,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="891" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A891" s="4">
         <v>1950</v>
       </c>
@@ -46284,7 +46296,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="892" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A892" s="4">
         <v>1950</v>
       </c>
@@ -46322,7 +46334,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="893" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A893" s="4">
         <v>1950</v>
       </c>
@@ -46360,7 +46372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="894" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A894" s="4">
         <v>1950</v>
       </c>
@@ -46398,7 +46410,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="895" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A895" s="4">
         <v>1950</v>
       </c>
@@ -46436,7 +46448,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="896" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A896" s="4">
         <v>1950</v>
       </c>
@@ -46474,7 +46486,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="897" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A897" s="4">
         <v>1950</v>
       </c>
@@ -46512,7 +46524,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="898" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A898" s="4">
         <v>1950</v>
       </c>
@@ -65166,6 +65178,9 @@
       <c r="K1388">
         <v>2</v>
       </c>
+      <c r="L1388" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="1389" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1389">
@@ -67667,6 +67682,12 @@
       </c>
       <c r="J1454" t="s">
         <v>88</v>
+      </c>
+      <c r="K1454">
+        <v>0</v>
+      </c>
+      <c r="L1454" t="s">
+        <v>3040</v>
       </c>
     </row>
     <row r="1455" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>